<commit_message>
Renamed and adjusted Motors
-Gibby
</commit_message>
<xml_diff>
--- a/Doc/Robot IO 2019.xlsx
+++ b/Doc/Robot IO 2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIRSTMentor\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIRSTMentor\Documents\GitHub\2019-Robot\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -375,49 +375,49 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,7 +703,7 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection sqref="A1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -712,618 +712,618 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="3"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="3"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="3"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="3"/>
+      <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>0</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7">
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5">
         <v>0</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="7">
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="5">
         <v>0</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="7">
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5">
         <v>0</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="Q5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R5" s="3"/>
+      <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="7">
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5">
         <v>1</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="7">
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="5">
         <v>1</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7">
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="5">
         <v>1</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="3"/>
+      <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="5">
+        <v>2</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="5">
+        <v>2</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="5">
+        <v>2</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5">
+        <v>3</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="5">
+        <v>3</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5">
+        <v>3</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5">
+        <v>4</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="5">
+        <v>4</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="D10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="5">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="5">
+        <v>5</v>
+      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5">
+        <v>6</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="5">
+        <v>6</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="7">
-        <v>2</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7">
-        <v>2</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="7">
-        <v>2</v>
-      </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="7">
-        <v>2</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="9" t="s">
+      <c r="F12" s="5">
+        <v>7</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5">
+        <v>7</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="5">
+        <v>7</v>
+      </c>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="7">
-        <v>3</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="7">
-        <v>3</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="7">
-        <v>3</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="7">
-        <v>3</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="7">
-        <v>4</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="7">
-        <v>4</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="7">
-        <v>4</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="7">
-        <v>5</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="7">
-        <v>5</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="7">
-        <v>5</v>
-      </c>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>7</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="7">
-        <v>6</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="7">
-        <v>6</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="7">
-        <v>6</v>
-      </c>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="F13" s="5">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5">
+        <v>8</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="5">
+        <v>8</v>
+      </c>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="9" t="s">
+      <c r="D14" s="12"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5">
+        <v>9</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5">
+        <v>9</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="5">
+        <v>9</v>
+      </c>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>12</v>
       </c>
-      <c r="F12" s="7">
-        <v>7</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="7">
-        <v>7</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="7">
-        <v>7</v>
-      </c>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>9</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="9" t="s">
+      <c r="B16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>13</v>
       </c>
-      <c r="F13" s="7">
-        <v>8</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="7">
-        <v>8</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="7">
-        <v>8</v>
-      </c>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="7">
-        <v>9</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="7">
-        <v>9</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="7">
-        <v>9</v>
-      </c>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
-        <v>11</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <v>12</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <v>13</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="3"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+      <c r="A18" s="5">
         <v>14</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
+      <c r="A19" s="8">
         <v>15</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="3"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="1"/>
     </row>
     <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
Disable arm current limiting (seems to help with resets).  Set up some hatch positions
</commit_message>
<xml_diff>
--- a/Doc/Robot IO 2019.xlsx
+++ b/Doc/Robot IO 2019.xlsx
@@ -148,10 +148,10 @@
     <t xml:space="preserve">Extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Intake</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cargo Intake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intake</t>
   </si>
 </sst>
 </file>
@@ -418,12 +418,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -968,7 +968,7 @@
       <c r="Q15" s="11"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="n">
         <v>12</v>
       </c>
@@ -992,7 +992,7 @@
       <c r="Q16" s="11"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="n">
         <v>13</v>
       </c>

</xml_diff>